<commit_message>
Se ceraron 3 test (unitaria, integración, extremo-extremo) para CierreMensualService , DeclaracioensRepositoryTest , ConfiguracionControllerTest
</commit_message>
<xml_diff>
--- a/backend/maven-demo/sisac_storage/declaraciones/Declaracion_202510_20123456789_BorradorCalculo.xlsx
+++ b/backend/maven-demo/sisac_storage/declaraciones/Declaracion_202510_20123456789_BorradorCalculo.xlsx
@@ -93,7 +93,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>196.2</v>
+        <v>333.0</v>
       </c>
     </row>
     <row r="3">
@@ -101,7 +101,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>126.0</v>
+        <v>255.66</v>
       </c>
     </row>
     <row r="4">
@@ -109,7 +109,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>70.2</v>
+        <v>77.34</v>
       </c>
     </row>
     <row r="5">
@@ -117,7 +117,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>19.29</v>
+        <v>32.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>